<commit_message>
Update proteome_limma_analysis (with column of new identifiers and removed old) 3.xlsx
</commit_message>
<xml_diff>
--- a/LA of proteome data/1st proteome LA results/proteome_limma_analysis (with column of new identifiers and removed old) 3.xlsx
+++ b/LA of proteome data/1st proteome LA results/proteome_limma_analysis (with column of new identifiers and removed old) 3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\R analysis of proteome data\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/LA of proteome data/1st proteome LA results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A30350-C29D-4DC5-9578-DD1EC5550D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E1A30350-C29D-4DC5-9578-DD1EC5550D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{765D033B-1632-4F24-A436-103A2D4FBF48}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1753,7 +1753,7 @@
   <dimension ref="A1:G303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>